<commit_message>
Bump to 0.2.0.  Added CommentTag, GroupTag, and HyperlinkTag.  Added Group functionality to looping tags.  Support Rich Text String formatting in certain appropriate tag attributes.  Added ExcelTransformer methods that accept input and output filenames.  Exposed JEXL cache and namespace functionality.  Fixed 2 bugs related to Formula parsing.  Added JUnit test cases for all parsers and all new tags.
</commit_message>
<xml_diff>
--- a/jett-core/templates/ExprTestTemplate.xlsx
+++ b/jett-core/templates/ExprTestTemplate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Cell A3</t>
   </si>
@@ -229,6 +229,18 @@
       </rPr>
       <t xml:space="preserve"> cell!</t>
     </r>
+  </si>
+  <si>
+    <t>Team:</t>
+  </si>
+  <si>
+    <t>${team}</t>
+  </si>
+  <si>
+    <t>List:</t>
+  </si>
+  <si>
+    <t>${numberList}</t>
   </si>
 </sst>
 </file>
@@ -660,6 +672,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
@@ -692,6 +712,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
@@ -707,6 +735,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ticket 46 - Added "fixed" attribute to "jt:span" tag.  If multiple blocks attempt to shift content out of the way inside a larger block, then the "jt:span" tag now has the option of not shifting redundantly.
</commit_message>
<xml_diff>
--- a/jett-core/templates/ExprTestTemplate.xlsx
+++ b/jett-core/templates/ExprTestTemplate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Cell A3</t>
   </si>
@@ -307,6 +307,18 @@
   </si>
   <si>
     <t>EscExprs:</t>
+  </si>
+  <si>
+    <t>Answer:</t>
+  </si>
+  <si>
+    <t>${answerToLifeTheUniverseAndEverything}</t>
+  </si>
+  <si>
+    <t>Pick A Card:</t>
+  </si>
+  <si>
+    <t>${jett:pickACard()}</t>
   </si>
 </sst>
 </file>
@@ -706,7 +718,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D30"/>
+  <dimension ref="A3:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -896,6 +908,22 @@
         <v>40</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>